<commit_message>
KIBON-2107: add lats betreuungsstunden prognose to statistik
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/LastenausgleichTagesschulen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/LastenausgleichTagesschulen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kibon\Dev\kiBon\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\new\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC303B01-0E23-4F14-81BB-00C6055A061B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13AC7733-CB59-4A5C-8EB1-B6C53AC64B8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gemeinden" sheetId="1" r:id="rId1"/>
@@ -187,9 +187,6 @@
     <t>1_Elterngebühren_Covid</t>
   </si>
   <si>
-    <t>1_Normlohnkosten_nichtpäd</t>
-  </si>
-  <si>
     <t>3_Betreuungsstunden_Prognose_kibon</t>
   </si>
   <si>
@@ -241,9 +238,6 @@
     <t>{betreuungsstundenNichtPaed}</t>
   </si>
   <si>
-    <t>{normlohnkostenNichtpaed}</t>
-  </si>
-  <si>
     <t>{elterngebuehrenBetreuung}</t>
   </si>
   <si>
@@ -362,6 +356,12 @@
   </si>
   <si>
     <t>{rowTagesschulenRepeat}</t>
+  </si>
+  <si>
+    <t>3_Betreuungsstunden_Prognose</t>
+  </si>
+  <si>
+    <t>{betreuungsstundenPrognose}</t>
   </si>
 </sst>
 </file>
@@ -406,7 +406,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -462,6 +462,19 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -476,22 +489,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -809,13 +822,13 @@
   <dimension ref="A1:AH8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="33" max="33" width="13.28515625" customWidth="1"/>
+    <col min="32" max="33" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="21" x14ac:dyDescent="0.35">
@@ -830,8 +843,8 @@
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>90</v>
+      <c r="B3" s="9" t="s">
+        <v>88</v>
       </c>
       <c r="C3" s="4"/>
     </row>
@@ -866,220 +879,221 @@
       <c r="AB6" s="11"/>
       <c r="AC6" s="11"/>
       <c r="AD6" s="11"/>
-      <c r="AE6" s="11"/>
-      <c r="AF6" s="11"/>
-      <c r="AG6" s="6" t="s">
+      <c r="AE6" s="12"/>
+      <c r="AF6" s="10" t="s">
         <v>51</v>
       </c>
+      <c r="AG6" s="12"/>
     </row>
-    <row r="7" spans="1:34" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:34" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="K7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="L7" s="7" t="s">
+      <c r="L7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="7" t="s">
+      <c r="M7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="N7" s="7" t="s">
+      <c r="N7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="O7" s="7" t="s">
+      <c r="O7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="R7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="S7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="T7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="U7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="V7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="W7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="X7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD7" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF7" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="P7" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q7" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="R7" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="S7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="T7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="U7" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="V7" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="W7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="X7" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y7" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z7" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA7" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB7" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC7" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD7" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE7" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF7" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG7" s="7" t="s">
-        <v>54</v>
+      <c r="AG7" s="6" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="L8" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="N8" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="N8" s="2" t="s">
+      <c r="O8" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="P8" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="P8" s="2" t="s">
+      <c r="Q8" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="Q8" s="2" t="s">
+      <c r="R8" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="R8" s="2" t="s">
+      <c r="S8" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="S8" s="2" t="s">
+      <c r="T8" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="T8" s="2" t="s">
+      <c r="U8" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="U8" s="2" t="s">
+      <c r="V8" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="V8" s="2" t="s">
+      <c r="W8" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="W8" s="2" t="s">
+      <c r="X8" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="X8" s="2" t="s">
+      <c r="Y8" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="Y8" s="2" t="s">
+      <c r="Z8" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="Z8" s="2" t="s">
+      <c r="AA8" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="AA8" s="2" t="s">
+      <c r="AB8" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="AB8" s="2" t="s">
+      <c r="AC8" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="AC8" s="2" t="s">
+      <c r="AD8" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="AD8" s="2" t="s">
+      <c r="AE8" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="AE8" s="2" t="s">
+      <c r="AF8" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="AF8" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="AG8" s="2" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="AH8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="F6:AF6"/>
+  <mergeCells count="2">
+    <mergeCell ref="AF6:AG6"/>
+    <mergeCell ref="F6:AE6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1097,130 +1111,130 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" s="7" t="s">
+      <c r="C1" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="R1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="S1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="T1" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="E2" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="U2" s="8" t="s">
         <v>109</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="U2" s="9" t="s">
-        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
KIBON-2481: Corona Frage ausblenden wenn nicht gesetzt, alle Texte Entfernen und die zwei spalten im Report ausblendet
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/LastenausgleichTagesschulen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/LastenausgleichTagesschulen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\new\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kibon\Dev\kiBon\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13AC7733-CB59-4A5C-8EB1-B6C53AC64B8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC888F09-2F2E-4DB5-B4D8-E521713C15AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gemeinden" sheetId="1" r:id="rId1"/>
@@ -499,10 +499,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -821,25 +821,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="32" max="33" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" customWidth="1"/>
+    <col min="16" max="17" width="0" hidden="1" customWidth="1"/>
+    <col min="32" max="33" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:34" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -848,44 +849,44 @@
       </c>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:34" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:34" ht="21" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="F6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="11"/>
-      <c r="U6" s="11"/>
-      <c r="V6" s="11"/>
-      <c r="W6" s="11"/>
-      <c r="X6" s="11"/>
-      <c r="Y6" s="11"/>
-      <c r="Z6" s="11"/>
-      <c r="AA6" s="11"/>
-      <c r="AB6" s="11"/>
-      <c r="AC6" s="11"/>
-      <c r="AD6" s="11"/>
-      <c r="AE6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
+      <c r="U6" s="12"/>
+      <c r="V6" s="12"/>
+      <c r="W6" s="12"/>
+      <c r="X6" s="12"/>
+      <c r="Y6" s="12"/>
+      <c r="Z6" s="12"/>
+      <c r="AA6" s="12"/>
+      <c r="AB6" s="12"/>
+      <c r="AC6" s="12"/>
+      <c r="AD6" s="12"/>
+      <c r="AE6" s="11"/>
       <c r="AF6" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="AG6" s="12"/>
+      <c r="AG6" s="11"/>
     </row>
-    <row r="7" spans="1:34" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
@@ -986,7 +987,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>56</v>
       </c>
@@ -1108,9 +1109,9 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>32</v>
       </c>
@@ -1172,7 +1173,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>89</v>
       </c>

</xml_diff>

<commit_message>
KIBON-2520: remove periode from report title
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/LastenausgleichTagesschulen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/LastenausgleichTagesschulen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kibon\Dev\kiBon\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\new\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC888F09-2F2E-4DB5-B4D8-E521713C15AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A08470-6322-4832-AEA3-04BEBE944451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gemeinden" sheetId="1" r:id="rId1"/>
@@ -43,9 +43,6 @@
     <t>0_Status</t>
   </si>
   <si>
-    <t>Lastenausgleich Tagesschulen 2020/21</t>
-  </si>
-  <si>
     <t>Angaben Gemeinde</t>
   </si>
   <si>
@@ -362,6 +359,9 @@
   </si>
   <si>
     <t>{betreuungsstundenPrognose}</t>
+  </si>
+  <si>
+    <t>Lastenausgleich Tagesschulen</t>
   </si>
 </sst>
 </file>
@@ -821,40 +821,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
     <col min="16" max="17" width="0" hidden="1" customWidth="1"/>
-    <col min="32" max="33" width="13.33203125" customWidth="1"/>
+    <col min="32" max="33" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:34" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:34" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:34" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:34" ht="21" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:34" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="F6" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
@@ -882,11 +880,11 @@
       <c r="AD6" s="12"/>
       <c r="AE6" s="11"/>
       <c r="AF6" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AG6" s="11"/>
     </row>
-    <row r="7" spans="1:34" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:34" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
@@ -894,7 +892,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>3</v>
@@ -903,192 +901,192 @@
         <v>4</v>
       </c>
       <c r="F7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="H7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="I7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="J7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="K7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="L7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="L7" s="6" t="s">
+      <c r="M7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="6" t="s">
+      <c r="N7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="N7" s="6" t="s">
+      <c r="O7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="O7" s="6" t="s">
+      <c r="P7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="P7" s="6" t="s">
+      <c r="Q7" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="R7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="Q7" s="6" t="s">
+      <c r="S7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="T7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="U7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="V7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="W7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="X7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE7" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF7" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="R7" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="S7" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="T7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="U7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="V7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="W7" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="X7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB7" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="AC7" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="AD7" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="AE7" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="AF7" s="6" t="s">
-        <v>53</v>
-      </c>
       <c r="AG7" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="U8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="V8" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="X8" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z8" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA8" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB8" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE8" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AF8" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="AG8" s="2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q8" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="R8" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="S8" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="T8" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="U8" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="V8" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="W8" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="X8" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="Y8" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="Z8" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="AA8" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AB8" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AC8" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="AD8" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="AE8" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AF8" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AG8" s="2" t="s">
-        <v>111</v>
-      </c>
       <c r="AH8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1109,133 +1107,133 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="T1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="T1" s="6" t="s">
-        <v>50</v>
-      </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" s="8" t="s">
         <v>108</v>
-      </c>
-      <c r="U2" s="8" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
KIBON-2626 add bemerkungen to excel
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/LastenausgleichTagesschulen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/LastenausgleichTagesschulen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\new\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A08470-6322-4832-AEA3-04BEBE944451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632F6FBF-3958-4597-96AF-F1444F9CB781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gemeinden" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="114">
   <si>
     <t>Datum generiert</t>
   </si>
@@ -362,6 +362,12 @@
   </si>
   <si>
     <t>Lastenausgleich Tagesschulen</t>
+  </si>
+  <si>
+    <t>3_Betreuungsstunden_Prognose_Bemerkungen</t>
+  </si>
+  <si>
+    <t>{betreuungsstundenPrognoseBemerkungen}</t>
   </si>
 </sst>
 </file>
@@ -481,7 +487,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -503,6 +509,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -819,7 +828,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH8"/>
+  <dimension ref="A1:AI8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -830,15 +839,15 @@
     <col min="32" max="33" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -847,10 +856,10 @@
       </c>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:34" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="F6" s="10" t="s">
         <v>5</v>
       </c>
@@ -879,12 +888,13 @@
       <c r="AC6" s="12"/>
       <c r="AD6" s="12"/>
       <c r="AE6" s="11"/>
-      <c r="AF6" s="10" t="s">
+      <c r="AF6" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="AG6" s="11"/>
+      <c r="AG6" s="13"/>
+      <c r="AH6" s="13"/>
     </row>
-    <row r="7" spans="1:34" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
@@ -984,8 +994,11 @@
       <c r="AG7" s="6" t="s">
         <v>109</v>
       </c>
+      <c r="AH7" s="6" t="s">
+        <v>112</v>
+      </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>55</v>
       </c>
@@ -1085,14 +1098,17 @@
       <c r="AG8" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="AH8" t="s">
+      <c r="AH8" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AI8" t="s">
         <v>54</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="AF6:AG6"/>
     <mergeCell ref="F6:AE6"/>
+    <mergeCell ref="AF6:AH6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-2625 add bemerkungen to excel
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/LastenausgleichTagesschulen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/LastenausgleichTagesschulen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\new\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A08470-6322-4832-AEA3-04BEBE944451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632F6FBF-3958-4597-96AF-F1444F9CB781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gemeinden" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="114">
   <si>
     <t>Datum generiert</t>
   </si>
@@ -362,6 +362,12 @@
   </si>
   <si>
     <t>Lastenausgleich Tagesschulen</t>
+  </si>
+  <si>
+    <t>3_Betreuungsstunden_Prognose_Bemerkungen</t>
+  </si>
+  <si>
+    <t>{betreuungsstundenPrognoseBemerkungen}</t>
   </si>
 </sst>
 </file>
@@ -481,7 +487,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -503,6 +509,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -819,7 +828,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH8"/>
+  <dimension ref="A1:AI8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -830,15 +839,15 @@
     <col min="32" max="33" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:34" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -847,10 +856,10 @@
       </c>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:34" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="F6" s="10" t="s">
         <v>5</v>
       </c>
@@ -879,12 +888,13 @@
       <c r="AC6" s="12"/>
       <c r="AD6" s="12"/>
       <c r="AE6" s="11"/>
-      <c r="AF6" s="10" t="s">
+      <c r="AF6" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="AG6" s="11"/>
+      <c r="AG6" s="13"/>
+      <c r="AH6" s="13"/>
     </row>
-    <row r="7" spans="1:34" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
@@ -984,8 +994,11 @@
       <c r="AG7" s="6" t="s">
         <v>109</v>
       </c>
+      <c r="AH7" s="6" t="s">
+        <v>112</v>
+      </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>55</v>
       </c>
@@ -1085,14 +1098,17 @@
       <c r="AG8" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="AH8" t="s">
+      <c r="AH8" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AI8" t="s">
         <v>54</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="AF6:AG6"/>
     <mergeCell ref="F6:AE6"/>
+    <mergeCell ref="AF6:AH6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-2653 add missing properties for lats report
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/LastenausgleichTagesschulen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/LastenausgleichTagesschulen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632F6FBF-3958-4597-96AF-F1444F9CB781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE0BF2B-89C3-4F20-BACA-CB6F2FA3F139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gemeinden" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="157">
   <si>
     <t>Datum generiert</t>
   </si>
@@ -142,9 +142,6 @@
     <t>2_Kinder_Sek</t>
   </si>
   <si>
-    <t>2_Kinder_Faktor</t>
-  </si>
-  <si>
     <t>2_Kinder_früh</t>
   </si>
   <si>
@@ -316,9 +313,6 @@
     <t>{kinderPrimar}</t>
   </si>
   <si>
-    <t>{kinderFaktor}</t>
-  </si>
-  <si>
     <t>{kinderFrueh}</t>
   </si>
   <si>
@@ -368,6 +362,141 @@
   </si>
   <si>
     <t>{betreuungsstundenPrognoseBemerkungen}</t>
+  </si>
+  <si>
+    <t>1_Betreuungsstunden_Faktor_3</t>
+  </si>
+  <si>
+    <t>{betreuungsstundenFaktor3}</t>
+  </si>
+  <si>
+    <t>2_Kinder_Faktor_1,5</t>
+  </si>
+  <si>
+    <t>2_Kinder_Faktor_3</t>
+  </si>
+  <si>
+    <t>{kinderFaktor15}</t>
+  </si>
+  <si>
+    <t>2_Früehbet_Mi</t>
+  </si>
+  <si>
+    <t>2_Früehbet_Di</t>
+  </si>
+  <si>
+    <t>2_Früehbet_Mo</t>
+  </si>
+  <si>
+    <t>2_Früehbet_Do</t>
+  </si>
+  <si>
+    <t>2_Früehbet_Fr</t>
+  </si>
+  <si>
+    <t>2_Mittagsbet_Mo</t>
+  </si>
+  <si>
+    <t>2_Mittagsbet_Di</t>
+  </si>
+  <si>
+    <t>2_Mittagsbet_Mi</t>
+  </si>
+  <si>
+    <t>2_Mittagsbet_Do</t>
+  </si>
+  <si>
+    <t>2_Mittagsbet_Fr</t>
+  </si>
+  <si>
+    <t>2_Nachmittagsbet_1_Mo</t>
+  </si>
+  <si>
+    <t>2_Nachmittagsbet_1_Di</t>
+  </si>
+  <si>
+    <t>2_Nachmittagsbet_1_Mi</t>
+  </si>
+  <si>
+    <t>2_Nachmittagsbet_1_Do</t>
+  </si>
+  <si>
+    <t>2_Nachmittagsbet_1_Fr</t>
+  </si>
+  <si>
+    <t>2_Nachmittagsbet_2_Mo</t>
+  </si>
+  <si>
+    <t>2_Nachmittagsbet_2_Di</t>
+  </si>
+  <si>
+    <t>2_Nachmittagsbet_2_Mi</t>
+  </si>
+  <si>
+    <t>2_Nachmittagsbet_2_Do</t>
+  </si>
+  <si>
+    <t>2_Nachmittagsbet_2_Fr</t>
+  </si>
+  <si>
+    <t>{fruehBetDi}</t>
+  </si>
+  <si>
+    <t>{fruehBetMo}</t>
+  </si>
+  <si>
+    <t>{fruehBetMi}</t>
+  </si>
+  <si>
+    <t>{fruehBetDo}</t>
+  </si>
+  <si>
+    <t>{fruehBetFr}</t>
+  </si>
+  <si>
+    <t>{mittagsBetMo}</t>
+  </si>
+  <si>
+    <t>{mittagsBetDi}</t>
+  </si>
+  <si>
+    <t>{mittagsBetMi}</t>
+  </si>
+  <si>
+    <t>{mittagsBetDo}</t>
+  </si>
+  <si>
+    <t>{mittagsBetFr}</t>
+  </si>
+  <si>
+    <t>{nachmittags1BetMo}</t>
+  </si>
+  <si>
+    <t>{nachmittags1BetDi}</t>
+  </si>
+  <si>
+    <t>{nachmittags1BetMi}</t>
+  </si>
+  <si>
+    <t>{nachmittags1BetDo}</t>
+  </si>
+  <si>
+    <t>{nachmittags1BetFr}</t>
+  </si>
+  <si>
+    <t>{nachmittags2BetMo}</t>
+  </si>
+  <si>
+    <t>{nachmittags2BetDi}</t>
+  </si>
+  <si>
+    <t>{nachmittags2BetMi}</t>
+  </si>
+  <si>
+    <t>{nachmittags2BetDo}</t>
+  </si>
+  <si>
+    <t>{nachmittags2BetFr}</t>
   </si>
 </sst>
 </file>
@@ -487,7 +616,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -505,14 +634,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -828,73 +960,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI8"/>
+  <dimension ref="A1:AJ8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="16" max="17" width="0" hidden="1" customWidth="1"/>
-    <col min="32" max="33" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" customWidth="1"/>
+    <col min="17" max="18" width="0" hidden="1" customWidth="1"/>
+    <col min="33" max="34" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:36" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:36" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:35" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:35" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:36" ht="21" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
       <c r="F6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="12"/>
-      <c r="T6" s="12"/>
-      <c r="U6" s="12"/>
-      <c r="V6" s="12"/>
-      <c r="W6" s="12"/>
-      <c r="X6" s="12"/>
-      <c r="Y6" s="12"/>
-      <c r="Z6" s="12"/>
-      <c r="AA6" s="12"/>
-      <c r="AB6" s="12"/>
-      <c r="AC6" s="12"/>
-      <c r="AD6" s="12"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="11"/>
+      <c r="AB6" s="11"/>
+      <c r="AC6" s="11"/>
+      <c r="AD6" s="11"/>
       <c r="AE6" s="11"/>
-      <c r="AF6" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="AG6" s="13"/>
+      <c r="AF6" s="12"/>
+      <c r="AG6" s="13" t="s">
+        <v>49</v>
+      </c>
       <c r="AH6" s="13"/>
+      <c r="AI6" s="13"/>
     </row>
-    <row r="7" spans="1:35" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
@@ -932,183 +1065,189 @@
         <v>12</v>
       </c>
       <c r="M7" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="N7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="N7" s="6" t="s">
+      <c r="O7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="O7" s="6" t="s">
+      <c r="P7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="P7" s="6" t="s">
+      <c r="Q7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="Q7" s="6" t="s">
+      <c r="R7" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="S7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="T7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="U7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="V7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="W7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="X7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF7" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG7" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="R7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="S7" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="T7" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="U7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="V7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="W7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="X7" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC7" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD7" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE7" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF7" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG7" s="6" t="s">
-        <v>109</v>
-      </c>
       <c r="AH7" s="6" t="s">
-        <v>112</v>
+        <v>107</v>
+      </c>
+      <c r="AI7" s="6" t="s">
+        <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="L8" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="M8" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="N8" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="O8" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="N8" s="2" t="s">
+      <c r="P8" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="Q8" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="P8" s="2" t="s">
+      <c r="R8" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="Q8" s="2" t="s">
+      <c r="S8" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="R8" s="2" t="s">
+      <c r="T8" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="S8" s="2" t="s">
+      <c r="U8" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="T8" s="2" t="s">
+      <c r="V8" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="U8" s="2" t="s">
+      <c r="W8" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="V8" s="2" t="s">
+      <c r="X8" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="W8" s="2" t="s">
+      <c r="Y8" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="X8" s="2" t="s">
+      <c r="Z8" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="Y8" s="2" t="s">
+      <c r="AA8" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="Z8" s="2" t="s">
+      <c r="AB8" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="AA8" s="2" t="s">
+      <c r="AC8" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="AB8" s="2" t="s">
+      <c r="AD8" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="AC8" s="2" t="s">
+      <c r="AE8" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="AD8" s="2" t="s">
+      <c r="AF8" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="AE8" s="2" t="s">
+      <c r="AG8" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="AF8" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AG8" s="2" t="s">
-        <v>110</v>
-      </c>
       <c r="AH8" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="AI8" t="s">
-        <v>54</v>
+        <v>108</v>
+      </c>
+      <c r="AI8" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="F6:AE6"/>
-    <mergeCell ref="AF6:AH6"/>
+    <mergeCell ref="F6:AF6"/>
+    <mergeCell ref="AG6:AI6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1117,15 +1256,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F13F8415-A30A-4B67-A28F-598A0482BFD0}">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:AP2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>31</v>
       </c>
@@ -1133,7 +1270,7 @@
         <v>32</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>33</v>
@@ -1151,108 +1288,235 @@
         <v>37</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="T1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="U1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="T1" s="6" t="s">
-        <v>49</v>
+      <c r="V1" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="W1" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="X1" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y1" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z1" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="AA1" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB1" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC1" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="AD1" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="AE1" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="AF1" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="AG1" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="AH1" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="AI1" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="AJ1" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="AK1" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="AL1" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="AM1" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="AN1" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="AO1" s="14" t="s">
+        <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="V2" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="AL2" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="AP2" s="8" t="s">
         <v>106</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="U2" s="8" t="s">
-        <v>108</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
KIBON-2653 fix wrong key in template
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/LastenausgleichTagesschulen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/LastenausgleichTagesschulen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE0BF2B-89C3-4F20-BACA-CB6F2FA3F139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D17977-05D5-4713-AE8D-AFE4F8311A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gemeinden" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="158">
   <si>
     <t>Datum generiert</t>
   </si>
@@ -497,6 +497,9 @@
   </si>
   <si>
     <t>{nachmittags2BetFr}</t>
+  </si>
+  <si>
+    <t>{kinderFaktor3}</t>
   </si>
 </sst>
 </file>
@@ -631,6 +634,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -642,9 +648,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -962,7 +965,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -992,40 +997,40 @@
       <c r="A4" s="1"/>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="11"/>
-      <c r="U6" s="11"/>
-      <c r="V6" s="11"/>
-      <c r="W6" s="11"/>
-      <c r="X6" s="11"/>
-      <c r="Y6" s="11"/>
-      <c r="Z6" s="11"/>
-      <c r="AA6" s="11"/>
-      <c r="AB6" s="11"/>
-      <c r="AC6" s="11"/>
-      <c r="AD6" s="11"/>
-      <c r="AE6" s="11"/>
-      <c r="AF6" s="12"/>
-      <c r="AG6" s="13" t="s">
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
+      <c r="U6" s="12"/>
+      <c r="V6" s="12"/>
+      <c r="W6" s="12"/>
+      <c r="X6" s="12"/>
+      <c r="Y6" s="12"/>
+      <c r="Z6" s="12"/>
+      <c r="AA6" s="12"/>
+      <c r="AB6" s="12"/>
+      <c r="AC6" s="12"/>
+      <c r="AD6" s="12"/>
+      <c r="AE6" s="12"/>
+      <c r="AF6" s="13"/>
+      <c r="AG6" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="AH6" s="13"/>
-      <c r="AI6" s="13"/>
+      <c r="AH6" s="14"/>
+      <c r="AI6" s="14"/>
     </row>
     <row r="7" spans="1:36" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
@@ -1258,7 +1263,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F13F8415-A30A-4B67-A28F-598A0482BFD0}">
   <dimension ref="A1:AP2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -1326,64 +1333,64 @@
       <c r="U1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="V1" s="14" t="s">
+      <c r="V1" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="W1" s="14" t="s">
+      <c r="W1" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="X1" s="14" t="s">
+      <c r="X1" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="Y1" s="14" t="s">
+      <c r="Y1" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="Z1" s="14" t="s">
+      <c r="Z1" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="AA1" s="14" t="s">
+      <c r="AA1" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="AB1" s="14" t="s">
+      <c r="AB1" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="AC1" s="14" t="s">
+      <c r="AC1" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="AD1" s="14" t="s">
+      <c r="AD1" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="AE1" s="14" t="s">
+      <c r="AE1" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="AF1" s="14" t="s">
+      <c r="AF1" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="AG1" s="14" t="s">
+      <c r="AG1" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="AH1" s="14" t="s">
+      <c r="AH1" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="AI1" s="14" t="s">
+      <c r="AI1" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="AJ1" s="14" t="s">
+      <c r="AJ1" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="AK1" s="14" t="s">
+      <c r="AK1" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="AL1" s="14" t="s">
+      <c r="AL1" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="AM1" s="14" t="s">
+      <c r="AM1" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="AN1" s="14" t="s">
+      <c r="AN1" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="AO1" s="14" t="s">
+      <c r="AO1" s="10" t="s">
         <v>136</v>
       </c>
     </row>
@@ -1416,7 +1423,7 @@
         <v>116</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>116</v>
+        <v>157</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>95</v>

</xml_diff>

<commit_message>
KIBON-2653 change active tab in template
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/LastenausgleichTagesschulen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/LastenausgleichTagesschulen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D17977-05D5-4713-AE8D-AFE4F8311A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5548A962-FBB7-4055-ACF5-D58AFB93C473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gemeinden" sheetId="1" r:id="rId1"/>
@@ -965,26 +965,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
     <col min="17" max="18" width="0" hidden="1" customWidth="1"/>
-    <col min="33" max="34" width="13.33203125" customWidth="1"/>
+    <col min="33" max="34" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:36" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:36" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -993,10 +991,10 @@
       </c>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:36" ht="21" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:36" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="F6" s="11" t="s">
         <v>5</v>
       </c>
@@ -1032,7 +1030,7 @@
       <c r="AH6" s="14"/>
       <c r="AI6" s="14"/>
     </row>
-    <row r="7" spans="1:36" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
@@ -1139,7 +1137,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>54</v>
       </c>
@@ -1263,13 +1261,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F13F8415-A30A-4B67-A28F-598A0482BFD0}">
   <dimension ref="A1:AP2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:42" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:42" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>31</v>
       </c>
@@ -1394,7 +1392,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>87</v>
       </c>

</xml_diff>

<commit_message>
KIBON-2653 add timestampMutiert to lats report
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/LastenausgleichTagesschulen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/LastenausgleichTagesschulen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5548A962-FBB7-4055-ACF5-D58AFB93C473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D45B60C-BF6F-4D9E-900D-92B4146DAF84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gemeinden" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="116">
   <si>
     <t>Datum generiert</t>
   </si>
@@ -142,6 +142,9 @@
     <t>2_Kinder_Sek</t>
   </si>
   <si>
+    <t>2_Kinder_Faktor</t>
+  </si>
+  <si>
     <t>2_Kinder_früh</t>
   </si>
   <si>
@@ -313,6 +316,9 @@
     <t>{kinderPrimar}</t>
   </si>
   <si>
+    <t>{kinderFaktor}</t>
+  </si>
+  <si>
     <t>{kinderFrueh}</t>
   </si>
   <si>
@@ -364,142 +370,10 @@
     <t>{betreuungsstundenPrognoseBemerkungen}</t>
   </si>
   <si>
-    <t>1_Betreuungsstunden_Faktor_3</t>
-  </si>
-  <si>
-    <t>{betreuungsstundenFaktor3}</t>
-  </si>
-  <si>
-    <t>2_Kinder_Faktor_1,5</t>
-  </si>
-  <si>
-    <t>2_Kinder_Faktor_3</t>
-  </si>
-  <si>
-    <t>{kinderFaktor15}</t>
-  </si>
-  <si>
-    <t>2_Früehbet_Mi</t>
-  </si>
-  <si>
-    <t>2_Früehbet_Di</t>
-  </si>
-  <si>
-    <t>2_Früehbet_Mo</t>
-  </si>
-  <si>
-    <t>2_Früehbet_Do</t>
-  </si>
-  <si>
-    <t>2_Früehbet_Fr</t>
-  </si>
-  <si>
-    <t>2_Mittagsbet_Mo</t>
-  </si>
-  <si>
-    <t>2_Mittagsbet_Di</t>
-  </si>
-  <si>
-    <t>2_Mittagsbet_Mi</t>
-  </si>
-  <si>
-    <t>2_Mittagsbet_Do</t>
-  </si>
-  <si>
-    <t>2_Mittagsbet_Fr</t>
-  </si>
-  <si>
-    <t>2_Nachmittagsbet_1_Mo</t>
-  </si>
-  <si>
-    <t>2_Nachmittagsbet_1_Di</t>
-  </si>
-  <si>
-    <t>2_Nachmittagsbet_1_Mi</t>
-  </si>
-  <si>
-    <t>2_Nachmittagsbet_1_Do</t>
-  </si>
-  <si>
-    <t>2_Nachmittagsbet_1_Fr</t>
-  </si>
-  <si>
-    <t>2_Nachmittagsbet_2_Mo</t>
-  </si>
-  <si>
-    <t>2_Nachmittagsbet_2_Di</t>
-  </si>
-  <si>
-    <t>2_Nachmittagsbet_2_Mi</t>
-  </si>
-  <si>
-    <t>2_Nachmittagsbet_2_Do</t>
-  </si>
-  <si>
-    <t>2_Nachmittagsbet_2_Fr</t>
-  </si>
-  <si>
-    <t>{fruehBetDi}</t>
-  </si>
-  <si>
-    <t>{fruehBetMo}</t>
-  </si>
-  <si>
-    <t>{fruehBetMi}</t>
-  </si>
-  <si>
-    <t>{fruehBetDo}</t>
-  </si>
-  <si>
-    <t>{fruehBetFr}</t>
-  </si>
-  <si>
-    <t>{mittagsBetMo}</t>
-  </si>
-  <si>
-    <t>{mittagsBetDi}</t>
-  </si>
-  <si>
-    <t>{mittagsBetMi}</t>
-  </si>
-  <si>
-    <t>{mittagsBetDo}</t>
-  </si>
-  <si>
-    <t>{mittagsBetFr}</t>
-  </si>
-  <si>
-    <t>{nachmittags1BetMo}</t>
-  </si>
-  <si>
-    <t>{nachmittags1BetDi}</t>
-  </si>
-  <si>
-    <t>{nachmittags1BetMi}</t>
-  </si>
-  <si>
-    <t>{nachmittags1BetDo}</t>
-  </si>
-  <si>
-    <t>{nachmittags1BetFr}</t>
-  </si>
-  <si>
-    <t>{nachmittags2BetMo}</t>
-  </si>
-  <si>
-    <t>{nachmittags2BetDi}</t>
-  </si>
-  <si>
-    <t>{nachmittags2BetMi}</t>
-  </si>
-  <si>
-    <t>{nachmittags2BetDo}</t>
-  </si>
-  <si>
-    <t>{nachmittags2BetFr}</t>
-  </si>
-  <si>
-    <t>{kinderFaktor3}</t>
+    <t>0_zuletzt_bearbeitet</t>
+  </si>
+  <si>
+    <t>{timestampMutiert}</t>
   </si>
 </sst>
 </file>
@@ -619,7 +493,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -634,9 +508,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -649,6 +520,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="22" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -967,70 +840,69 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" customWidth="1"/>
     <col min="17" max="18" width="0" hidden="1" customWidth="1"/>
-    <col min="33" max="34" width="13.28515625" customWidth="1"/>
+    <col min="33" max="34" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:36" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:36" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:36" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:36" ht="21" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="F6" s="11" t="s">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="G6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="12"/>
-      <c r="T6" s="12"/>
-      <c r="U6" s="12"/>
-      <c r="V6" s="12"/>
-      <c r="W6" s="12"/>
-      <c r="X6" s="12"/>
-      <c r="Y6" s="12"/>
-      <c r="Z6" s="12"/>
-      <c r="AA6" s="12"/>
-      <c r="AB6" s="12"/>
-      <c r="AC6" s="12"/>
-      <c r="AD6" s="12"/>
-      <c r="AE6" s="12"/>
-      <c r="AF6" s="13"/>
-      <c r="AG6" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="AH6" s="14"/>
-      <c r="AI6" s="14"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
+      <c r="V6" s="11"/>
+      <c r="W6" s="11"/>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="11"/>
+      <c r="AB6" s="11"/>
+      <c r="AC6" s="11"/>
+      <c r="AD6" s="11"/>
+      <c r="AE6" s="11"/>
+      <c r="AF6" s="12"/>
+      <c r="AG6" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH6" s="13"/>
+      <c r="AI6" s="13"/>
     </row>
-    <row r="7" spans="1:36" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
@@ -1046,29 +918,29 @@
       <c r="E7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="G7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="H7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="I7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="J7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="K7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="L7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="L7" s="6" t="s">
+      <c r="M7" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>112</v>
       </c>
       <c r="N7" s="6" t="s">
         <v>13</v>
@@ -1083,7 +955,7 @@
         <v>16</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="S7" s="6" t="s">
         <v>17</v>
@@ -1128,33 +1000,33 @@
         <v>30</v>
       </c>
       <c r="AG7" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AH7" s="6" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="AI7" s="6" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F8" s="2" t="s">
         <v>59</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>115</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>60</v>
@@ -1175,81 +1047,81 @@
         <v>65</v>
       </c>
       <c r="M8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="U8" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="V8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="X8" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y8" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA8" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB8" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC8" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AE8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF8" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG8" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="AH8" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI8" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="N8" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q8" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="R8" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="S8" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="T8" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="U8" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="V8" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="W8" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="X8" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y8" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="Z8" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA8" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AB8" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="AC8" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="AD8" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE8" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AF8" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="AG8" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="AH8" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="AI8" s="2" t="s">
-        <v>111</v>
-      </c>
       <c r="AJ8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="F6:AF6"/>
+    <mergeCell ref="G6:AF6"/>
     <mergeCell ref="AG6:AI6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1259,15 +1131,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F13F8415-A30A-4B67-A28F-598A0482BFD0}">
-  <dimension ref="A1:AP2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:42" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>31</v>
       </c>
@@ -1275,7 +1147,7 @@
         <v>32</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>33</v>
@@ -1293,235 +1165,108 @@
         <v>37</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>114</v>
+        <v>38</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>115</v>
+        <v>39</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="U1" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="V1" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="W1" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="X1" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="Y1" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="Z1" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="AA1" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="AB1" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="AC1" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="AD1" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="AE1" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="AF1" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="AG1" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="AH1" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="AI1" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="AJ1" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="AK1" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="AL1" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="AM1" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="AN1" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="AO1" s="10" t="s">
-        <v>136</v>
+        <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>93</v>
-      </c>
       <c r="I2" s="2" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>157</v>
+        <v>97</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="AG2" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="AH2" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="AI2" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="AK2" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="AL2" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="AM2" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="AN2" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="AO2" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="AP2" s="8" t="s">
-        <v>106</v>
+        <v>107</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
KIBON-2653 make timestamp column wider
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/LastenausgleichTagesschulen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/LastenausgleichTagesschulen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D45B60C-BF6F-4D9E-900D-92B4146DAF84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58042792-514E-4E1B-BC32-A5F417A2E8BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -508,6 +508,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -520,8 +522,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -843,6 +843,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.6640625" customWidth="1"/>
+    <col min="6" max="6" width="18.5546875" customWidth="1"/>
     <col min="17" max="18" width="0" hidden="1" customWidth="1"/>
     <col min="33" max="34" width="13.33203125" customWidth="1"/>
   </cols>
@@ -868,39 +869,39 @@
       <c r="A4" s="1"/>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="11"/>
-      <c r="U6" s="11"/>
-      <c r="V6" s="11"/>
-      <c r="W6" s="11"/>
-      <c r="X6" s="11"/>
-      <c r="Y6" s="11"/>
-      <c r="Z6" s="11"/>
-      <c r="AA6" s="11"/>
-      <c r="AB6" s="11"/>
-      <c r="AC6" s="11"/>
-      <c r="AD6" s="11"/>
-      <c r="AE6" s="11"/>
-      <c r="AF6" s="12"/>
-      <c r="AG6" s="13" t="s">
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="13"/>
+      <c r="U6" s="13"/>
+      <c r="V6" s="13"/>
+      <c r="W6" s="13"/>
+      <c r="X6" s="13"/>
+      <c r="Y6" s="13"/>
+      <c r="Z6" s="13"/>
+      <c r="AA6" s="13"/>
+      <c r="AB6" s="13"/>
+      <c r="AC6" s="13"/>
+      <c r="AD6" s="13"/>
+      <c r="AE6" s="13"/>
+      <c r="AF6" s="14"/>
+      <c r="AG6" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="AH6" s="13"/>
-      <c r="AI6" s="13"/>
+      <c r="AH6" s="15"/>
+      <c r="AI6" s="15"/>
     </row>
     <row r="7" spans="1:36" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
@@ -918,7 +919,7 @@
       <c r="E7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="10" t="s">
         <v>114</v>
       </c>
       <c r="G7" s="6" t="s">
@@ -1025,7 +1026,7 @@
       <c r="E8" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="11" t="s">
         <v>115</v>
       </c>
       <c r="G8" s="2" t="s">

</xml_diff>

<commit_message>
KIBON-2653: Change Column kinderFaktor LATS Statistik
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/LastenausgleichTagesschulen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/LastenausgleichTagesschulen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58042792-514E-4E1B-BC32-A5F417A2E8BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BDB8E8-10CB-4FBA-AADD-996FABD7A21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gemeinden" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="118">
   <si>
     <t>Datum generiert</t>
   </si>
@@ -142,9 +142,6 @@
     <t>2_Kinder_Sek</t>
   </si>
   <si>
-    <t>2_Kinder_Faktor</t>
-  </si>
-  <si>
     <t>2_Kinder_früh</t>
   </si>
   <si>
@@ -316,9 +313,6 @@
     <t>{kinderPrimar}</t>
   </si>
   <si>
-    <t>{kinderFaktor}</t>
-  </si>
-  <si>
     <t>{kinderFrueh}</t>
   </si>
   <si>
@@ -374,6 +368,18 @@
   </si>
   <si>
     <t>{timestampMutiert}</t>
+  </si>
+  <si>
+    <t>{kinderFaktor3}</t>
+  </si>
+  <si>
+    <t>{kinderFaktor15}</t>
+  </si>
+  <si>
+    <t>2_Kinder_Faktor_3</t>
+  </si>
+  <si>
+    <t>2_Kinder_Faktor_15</t>
   </si>
 </sst>
 </file>
@@ -838,7 +844,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -850,7 +858,7 @@
   <sheetData>
     <row r="1" spans="1:36" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:36" ht="21" x14ac:dyDescent="0.4">
@@ -861,7 +869,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C3" s="4"/>
     </row>
@@ -898,7 +906,7 @@
       <c r="AE6" s="13"/>
       <c r="AF6" s="14"/>
       <c r="AG6" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AH6" s="15"/>
       <c r="AI6" s="15"/>
@@ -920,7 +928,7 @@
         <v>4</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>6</v>
@@ -956,7 +964,7 @@
         <v>16</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="S7" s="6" t="s">
         <v>17</v>
@@ -1001,123 +1009,123 @@
         <v>30</v>
       </c>
       <c r="AG7" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AH7" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="AI7" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F8" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="L8" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="N8" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="N8" s="2" t="s">
+      <c r="O8" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="P8" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="P8" s="2" t="s">
+      <c r="Q8" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="Q8" s="2" t="s">
+      <c r="R8" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="R8" s="2" t="s">
+      <c r="S8" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="S8" s="2" t="s">
+      <c r="T8" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="T8" s="2" t="s">
+      <c r="U8" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="U8" s="2" t="s">
+      <c r="V8" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="V8" s="2" t="s">
+      <c r="W8" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="W8" s="2" t="s">
+      <c r="X8" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="X8" s="2" t="s">
+      <c r="Y8" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="Y8" s="2" t="s">
+      <c r="Z8" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="Z8" s="2" t="s">
+      <c r="AA8" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AA8" s="2" t="s">
+      <c r="AB8" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="AB8" s="2" t="s">
+      <c r="AC8" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="AC8" s="2" t="s">
+      <c r="AD8" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="AD8" s="2" t="s">
+      <c r="AE8" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="AE8" s="2" t="s">
+      <c r="AF8" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="AF8" s="2" t="s">
+      <c r="AG8" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="AG8" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="AH8" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="AI8" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="AJ8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1132,15 +1140,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F13F8415-A30A-4B67-A28F-598A0482BFD0}">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>31</v>
       </c>
@@ -1148,7 +1156,7 @@
         <v>32</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>33</v>
@@ -1166,105 +1174,111 @@
         <v>37</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="T1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="U1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="T1" s="6" t="s">
-        <v>49</v>
-      </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="V2" s="8" t="s">
         <v>106</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="U2" s="8" t="s">
-        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
KIBON-2653 add oeffnungszeiten again
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/LastenausgleichTagesschulen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/LastenausgleichTagesschulen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BDB8E8-10CB-4FBA-AADD-996FABD7A21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E0AE64-DE1D-4717-BFF5-EFE75134BCF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gemeinden" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="158">
   <si>
     <t>Datum generiert</t>
   </si>
@@ -380,6 +380,126 @@
   </si>
   <si>
     <t>2_Kinder_Faktor_15</t>
+  </si>
+  <si>
+    <t>2_Früehbet_Mo</t>
+  </si>
+  <si>
+    <t>2_Früehbet_Di</t>
+  </si>
+  <si>
+    <t>2_Früehbet_Mi</t>
+  </si>
+  <si>
+    <t>2_Früehbet_Do</t>
+  </si>
+  <si>
+    <t>2_Früehbet_Fr</t>
+  </si>
+  <si>
+    <t>2_Mittagsbet_Mo</t>
+  </si>
+  <si>
+    <t>2_Mittagsbet_Di</t>
+  </si>
+  <si>
+    <t>2_Mittagsbet_Mi</t>
+  </si>
+  <si>
+    <t>2_Mittagsbet_Do</t>
+  </si>
+  <si>
+    <t>2_Mittagsbet_Fr</t>
+  </si>
+  <si>
+    <t>2_Nachmittagsbet_1_Mo</t>
+  </si>
+  <si>
+    <t>2_Nachmittagsbet_1_Di</t>
+  </si>
+  <si>
+    <t>2_Nachmittagsbet_1_Mi</t>
+  </si>
+  <si>
+    <t>2_Nachmittagsbet_1_Do</t>
+  </si>
+  <si>
+    <t>2_Nachmittagsbet_1_Fr</t>
+  </si>
+  <si>
+    <t>2_Nachmittagsbet_2_Mo</t>
+  </si>
+  <si>
+    <t>2_Nachmittagsbet_2_Di</t>
+  </si>
+  <si>
+    <t>2_Nachmittagsbet_2_Mi</t>
+  </si>
+  <si>
+    <t>2_Nachmittagsbet_2_Do</t>
+  </si>
+  <si>
+    <t>2_Nachmittagsbet_2_Fr</t>
+  </si>
+  <si>
+    <t>{fruehBetMo}</t>
+  </si>
+  <si>
+    <t>{fruehBetDi}</t>
+  </si>
+  <si>
+    <t>{fruehBetMi}</t>
+  </si>
+  <si>
+    <t>{fruehBetDo}</t>
+  </si>
+  <si>
+    <t>{fruehBetFr}</t>
+  </si>
+  <si>
+    <t>{mittagsBetMo}</t>
+  </si>
+  <si>
+    <t>{mittagsBetDi}</t>
+  </si>
+  <si>
+    <t>{mittagsBetMi}</t>
+  </si>
+  <si>
+    <t>{mittagsBetDo}</t>
+  </si>
+  <si>
+    <t>{mittagsBetFr}</t>
+  </si>
+  <si>
+    <t>{nachmittags1BetMo}</t>
+  </si>
+  <si>
+    <t>{nachmittags1BetDi}</t>
+  </si>
+  <si>
+    <t>{nachmittags1BetMi}</t>
+  </si>
+  <si>
+    <t>{nachmittags1BetDo}</t>
+  </si>
+  <si>
+    <t>{nachmittags1BetFr}</t>
+  </si>
+  <si>
+    <t>{nachmittags2BetMo}</t>
+  </si>
+  <si>
+    <t>{nachmittags2BetDi}</t>
+  </si>
+  <si>
+    <t>{nachmittags2BetMi}</t>
+  </si>
+  <si>
+    <t>{nachmittags2BetDo}</t>
+  </si>
+  <si>
+    <t>{nachmittags2BetFr}</t>
   </si>
 </sst>
 </file>
@@ -499,7 +619,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -527,6 +647,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -844,27 +967,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" customWidth="1"/>
-    <col min="6" max="6" width="18.5546875" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" customWidth="1"/>
     <col min="17" max="18" width="0" hidden="1" customWidth="1"/>
-    <col min="33" max="34" width="13.33203125" customWidth="1"/>
+    <col min="33" max="34" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:36" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:36" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -873,10 +994,10 @@
       </c>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:36" ht="21" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:36" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="G6" s="12" t="s">
         <v>5</v>
       </c>
@@ -911,7 +1032,7 @@
       <c r="AH6" s="15"/>
       <c r="AI6" s="15"/>
     </row>
-    <row r="7" spans="1:36" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
@@ -1018,7 +1139,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>54</v>
       </c>
@@ -1140,15 +1261,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F13F8415-A30A-4B67-A28F-598A0482BFD0}">
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:AP2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:42" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>31</v>
       </c>
@@ -1212,8 +1331,68 @@
       <c r="U1" s="6" t="s">
         <v>48</v>
       </c>
+      <c r="V1" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="W1" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="X1" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y1" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="Z1" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA1" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="AB1" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="AC1" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="AD1" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="AE1" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="AF1" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="AG1" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="AH1" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="AI1" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="AJ1" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="AK1" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="AL1" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="AM1" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="AN1" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="AO1" s="16" t="s">
+        <v>137</v>
+      </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>87</v>
       </c>
@@ -1277,7 +1456,67 @@
       <c r="U2" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="V2" s="8" t="s">
+      <c r="V2" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="AL2" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="AN2" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="AP2" s="8" t="s">
         <v>106</v>
       </c>
     </row>

</xml_diff>

<commit_message>
KIBON-2653 add other columns again
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/LastenausgleichTagesschulen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/LastenausgleichTagesschulen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E0AE64-DE1D-4717-BFF5-EFE75134BCF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E50D9D6-D1C9-401B-86D3-C1D8942EF36F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,17 +16,28 @@
     <sheet name="Gemeinden" sheetId="1" r:id="rId1"/>
     <sheet name="Tagesschulen" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="160">
   <si>
     <t>Datum generiert</t>
   </si>
@@ -500,6 +511,12 @@
   </si>
   <si>
     <t>{nachmittags2BetFr}</t>
+  </si>
+  <si>
+    <t>{betreuungsstundenFaktor3}</t>
+  </si>
+  <si>
+    <t>1_Betreuungsstunden_Faktor_3</t>
   </si>
 </sst>
 </file>
@@ -636,6 +653,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -647,9 +667,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -965,7 +982,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ8"/>
+  <dimension ref="A1:AK8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -973,19 +990,19 @@
   <cols>
     <col min="1" max="1" width="26.7109375" customWidth="1"/>
     <col min="6" max="6" width="18.5703125" customWidth="1"/>
-    <col min="17" max="18" width="0" hidden="1" customWidth="1"/>
-    <col min="33" max="34" width="13.28515625" customWidth="1"/>
+    <col min="18" max="19" width="0" hidden="1" customWidth="1"/>
+    <col min="34" max="35" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:37" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -994,45 +1011,46 @@
       </c>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:36" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:37" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="G6" s="12" t="s">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="G6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="13"/>
-      <c r="S6" s="13"/>
-      <c r="T6" s="13"/>
-      <c r="U6" s="13"/>
-      <c r="V6" s="13"/>
-      <c r="W6" s="13"/>
-      <c r="X6" s="13"/>
-      <c r="Y6" s="13"/>
-      <c r="Z6" s="13"/>
-      <c r="AA6" s="13"/>
-      <c r="AB6" s="13"/>
-      <c r="AC6" s="13"/>
-      <c r="AD6" s="13"/>
-      <c r="AE6" s="13"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14"/>
+      <c r="T6" s="14"/>
+      <c r="U6" s="14"/>
+      <c r="V6" s="14"/>
+      <c r="W6" s="14"/>
+      <c r="X6" s="14"/>
+      <c r="Y6" s="14"/>
+      <c r="Z6" s="14"/>
+      <c r="AA6" s="14"/>
+      <c r="AB6" s="14"/>
+      <c r="AC6" s="14"/>
+      <c r="AD6" s="14"/>
+      <c r="AE6" s="14"/>
       <c r="AF6" s="14"/>
-      <c r="AG6" s="15" t="s">
+      <c r="AG6" s="15"/>
+      <c r="AH6" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="AH6" s="15"/>
-      <c r="AI6" s="15"/>
+      <c r="AI6" s="16"/>
+      <c r="AJ6" s="16"/>
     </row>
-    <row r="7" spans="1:36" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
@@ -1073,73 +1091,76 @@
         <v>12</v>
       </c>
       <c r="N7" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="O7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="O7" s="6" t="s">
+      <c r="P7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P7" s="6" t="s">
+      <c r="Q7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="Q7" s="6" t="s">
+      <c r="R7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="R7" s="6" t="s">
+      <c r="S7" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="S7" s="6" t="s">
+      <c r="T7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="T7" s="6" t="s">
+      <c r="U7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="U7" s="6" t="s">
+      <c r="V7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="V7" s="6" t="s">
+      <c r="W7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="W7" s="6" t="s">
+      <c r="X7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="X7" s="6" t="s">
+      <c r="Y7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Y7" s="6" t="s">
+      <c r="Z7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="Z7" s="6" t="s">
+      <c r="AA7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="AA7" s="6" t="s">
+      <c r="AB7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="AB7" s="6" t="s">
+      <c r="AC7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="AC7" s="6" t="s">
+      <c r="AD7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="AD7" s="6" t="s">
+      <c r="AE7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="AE7" s="6" t="s">
+      <c r="AF7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="AF7" s="6" t="s">
+      <c r="AG7" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="AG7" s="6" t="s">
+      <c r="AH7" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AH7" s="6" t="s">
+      <c r="AI7" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="AI7" s="6" t="s">
+      <c r="AJ7" s="6" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>54</v>
       </c>
@@ -1180,79 +1201,82 @@
         <v>65</v>
       </c>
       <c r="N8" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="O8" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="P8" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="P8" s="2" t="s">
+      <c r="Q8" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="Q8" s="2" t="s">
+      <c r="R8" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="R8" s="2" t="s">
+      <c r="S8" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="S8" s="2" t="s">
+      <c r="T8" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="T8" s="2" t="s">
+      <c r="U8" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="U8" s="2" t="s">
+      <c r="V8" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="V8" s="2" t="s">
+      <c r="W8" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="W8" s="2" t="s">
+      <c r="X8" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="X8" s="2" t="s">
+      <c r="Y8" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="Y8" s="2" t="s">
+      <c r="Z8" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="Z8" s="2" t="s">
+      <c r="AA8" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AA8" s="2" t="s">
+      <c r="AB8" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AB8" s="2" t="s">
+      <c r="AC8" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="AC8" s="2" t="s">
+      <c r="AD8" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="AD8" s="2" t="s">
+      <c r="AE8" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="AE8" s="2" t="s">
+      <c r="AF8" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="AF8" s="2" t="s">
+      <c r="AG8" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="AG8" s="2" t="s">
+      <c r="AH8" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="AH8" s="2" t="s">
+      <c r="AI8" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="AI8" s="2" t="s">
+      <c r="AJ8" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="AJ8" t="s">
+      <c r="AK8" t="s">
         <v>53</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="G6:AF6"/>
-    <mergeCell ref="AG6:AI6"/>
+    <mergeCell ref="G6:AG6"/>
+    <mergeCell ref="AH6:AJ6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1293,10 +1317,10 @@
         <v>37</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>116</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>117</v>
       </c>
       <c r="K1" s="6" t="s">
         <v>38</v>
@@ -1331,64 +1355,64 @@
       <c r="U1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="V1" s="16" t="s">
+      <c r="V1" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="W1" s="16" t="s">
+      <c r="W1" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="X1" s="16" t="s">
+      <c r="X1" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="Y1" s="16" t="s">
+      <c r="Y1" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="Z1" s="16" t="s">
+      <c r="Z1" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="AA1" s="16" t="s">
+      <c r="AA1" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="AB1" s="16" t="s">
+      <c r="AB1" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="AC1" s="16" t="s">
+      <c r="AC1" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="AD1" s="16" t="s">
+      <c r="AD1" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="AE1" s="16" t="s">
+      <c r="AE1" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="AF1" s="16" t="s">
+      <c r="AF1" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="AG1" s="16" t="s">
+      <c r="AG1" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="AH1" s="16" t="s">
+      <c r="AH1" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="AI1" s="16" t="s">
+      <c r="AI1" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="AJ1" s="16" t="s">
+      <c r="AJ1" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="AK1" s="16" t="s">
+      <c r="AK1" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="AL1" s="16" t="s">
+      <c r="AL1" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="AM1" s="16" t="s">
+      <c r="AM1" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="AN1" s="16" t="s">
+      <c r="AN1" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="AO1" s="16" t="s">
+      <c r="AO1" s="12" t="s">
         <v>137</v>
       </c>
     </row>
@@ -1418,10 +1442,10 @@
         <v>93</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>115</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>95</v>

</xml_diff>

<commit_message>
KIBON-3041 neue felder in statistik aufnehmen
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/LastenausgleichTagesschulen.xlsx
+++ b/ebegu-server/src/main/resources/reporting/LastenausgleichTagesschulen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\kibon-app\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E50D9D6-D1C9-401B-86D3-C1D8942EF36F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B08114CC-2558-4965-9FEF-FC21346ECF25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gemeinden" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="168">
   <si>
     <t>Datum generiert</t>
   </si>
@@ -517,13 +517,37 @@
   </si>
   <si>
     <t>1_Betreuungsstunden_Faktor_3</t>
+  </si>
+  <si>
+    <t>2_Kinder_KinderBasisstufe</t>
+  </si>
+  <si>
+    <t>{kinderBasisstufe}</t>
+  </si>
+  <si>
+    <t>1_Elterngebühren_Volksschulangebot</t>
+  </si>
+  <si>
+    <t>{elterngebuehrenVolksschulangebot}</t>
+  </si>
+  <si>
+    <t>1_Bemerkungen_StarkeVeraenderung</t>
+  </si>
+  <si>
+    <t>{bemerkungStarkeVeraenderung}</t>
+  </si>
+  <si>
+    <t>1_Bemerkungen_Mindestens50ProzentAusgebildet</t>
+  </si>
+  <si>
+    <t>{bemerkungMindestens50ProzentAusgebildet}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -542,6 +566,12 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -636,20 +666,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -982,185 +1010,198 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AK8"/>
+  <dimension ref="A1:AN8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.7109375" customWidth="1"/>
     <col min="6" max="6" width="18.5703125" customWidth="1"/>
     <col min="18" max="19" width="0" hidden="1" customWidth="1"/>
-    <col min="34" max="35" width="13.28515625" customWidth="1"/>
+    <col min="37" max="38" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:40" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:40" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:37" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:40" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="G6" s="13" t="s">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="G6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="14"/>
-      <c r="S6" s="14"/>
-      <c r="T6" s="14"/>
-      <c r="U6" s="14"/>
-      <c r="V6" s="14"/>
-      <c r="W6" s="14"/>
-      <c r="X6" s="14"/>
-      <c r="Y6" s="14"/>
-      <c r="Z6" s="14"/>
-      <c r="AA6" s="14"/>
-      <c r="AB6" s="14"/>
-      <c r="AC6" s="14"/>
-      <c r="AD6" s="14"/>
-      <c r="AE6" s="14"/>
-      <c r="AF6" s="14"/>
-      <c r="AG6" s="15"/>
-      <c r="AH6" s="16" t="s">
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
+      <c r="U6" s="12"/>
+      <c r="V6" s="12"/>
+      <c r="W6" s="12"/>
+      <c r="X6" s="12"/>
+      <c r="Y6" s="12"/>
+      <c r="Z6" s="12"/>
+      <c r="AA6" s="12"/>
+      <c r="AB6" s="12"/>
+      <c r="AC6" s="12"/>
+      <c r="AD6" s="12"/>
+      <c r="AE6" s="12"/>
+      <c r="AF6" s="12"/>
+      <c r="AG6" s="12"/>
+      <c r="AH6" s="12"/>
+      <c r="AI6" s="12"/>
+      <c r="AJ6" s="13"/>
+      <c r="AK6" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="AI6" s="16"/>
-      <c r="AJ6" s="16"/>
+      <c r="AL6" s="14"/>
+      <c r="AM6" s="14"/>
     </row>
-    <row r="7" spans="1:37" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:40" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="J7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="K7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L7" s="6" t="s">
+      <c r="L7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M7" s="6" t="s">
+      <c r="M7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N7" s="6" t="s">
+      <c r="N7" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="O7" s="6" t="s">
+      <c r="O7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P7" s="6" t="s">
+      <c r="P7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q7" s="6" t="s">
+      <c r="Q7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="R7" s="6" t="s">
+      <c r="R7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="S7" s="6" t="s">
+      <c r="S7" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="T7" s="6" t="s">
+      <c r="T7" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="U7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="U7" s="6" t="s">
+      <c r="V7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="V7" s="6" t="s">
+      <c r="W7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="W7" s="6" t="s">
+      <c r="X7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="X7" s="6" t="s">
+      <c r="Y7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="Y7" s="6" t="s">
+      <c r="Z7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="Z7" s="6" t="s">
+      <c r="AA7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="AA7" s="6" t="s">
+      <c r="AB7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="AB7" s="6" t="s">
+      <c r="AC7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AC7" s="6" t="s">
+      <c r="AD7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AD7" s="6" t="s">
+      <c r="AE7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AE7" s="6" t="s">
+      <c r="AF7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AF7" s="6" t="s">
+      <c r="AG7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AG7" s="6" t="s">
+      <c r="AH7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AH7" s="6" t="s">
+      <c r="AI7" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="AJ7" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="AK7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AI7" s="6" t="s">
+      <c r="AL7" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="AJ7" s="6" t="s">
+      <c r="AM7" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>54</v>
       </c>
@@ -1176,7 +1217,7 @@
       <c r="E8" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="9" t="s">
         <v>113</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -1219,64 +1260,73 @@
         <v>70</v>
       </c>
       <c r="T8" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="U8" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="U8" s="2" t="s">
+      <c r="V8" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="V8" s="2" t="s">
+      <c r="W8" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="W8" s="2" t="s">
+      <c r="X8" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="X8" s="2" t="s">
+      <c r="Y8" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="Y8" s="2" t="s">
+      <c r="Z8" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="Z8" s="2" t="s">
+      <c r="AA8" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="AA8" s="2" t="s">
+      <c r="AB8" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AB8" s="2" t="s">
+      <c r="AC8" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AC8" s="2" t="s">
+      <c r="AD8" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="AD8" s="2" t="s">
+      <c r="AE8" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="AE8" s="2" t="s">
+      <c r="AF8" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="AF8" s="2" t="s">
+      <c r="AG8" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="AG8" s="2" t="s">
+      <c r="AH8" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="AH8" s="2" t="s">
+      <c r="AI8" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="AJ8" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="AK8" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="AI8" s="2" t="s">
+      <c r="AL8" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="AJ8" s="2" t="s">
+      <c r="AM8" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="AK8" t="s">
+      <c r="AN8" t="s">
         <v>53</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="G6:AG6"/>
-    <mergeCell ref="AH6:AJ6"/>
+    <mergeCell ref="AK6:AM6"/>
+    <mergeCell ref="G6:AJ6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1285,145 +1335,150 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F13F8415-A30A-4B67-A28F-598A0482BFD0}">
-  <dimension ref="A1:AP2"/>
+  <dimension ref="A1:AQ2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:42" ht="60" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:43" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="P1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="R1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="S1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="T1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="U1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="V1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="V1" s="12" t="s">
+      <c r="W1" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="W1" s="12" t="s">
+      <c r="X1" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="X1" s="12" t="s">
+      <c r="Y1" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="Y1" s="12" t="s">
+      <c r="Z1" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="Z1" s="12" t="s">
+      <c r="AA1" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="AA1" s="12" t="s">
+      <c r="AB1" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="AB1" s="12" t="s">
+      <c r="AC1" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="AC1" s="12" t="s">
+      <c r="AD1" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="AD1" s="12" t="s">
+      <c r="AE1" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="AE1" s="12" t="s">
+      <c r="AF1" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="AF1" s="12" t="s">
+      <c r="AG1" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="AG1" s="12" t="s">
+      <c r="AH1" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="AH1" s="12" t="s">
+      <c r="AI1" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="AI1" s="12" t="s">
+      <c r="AJ1" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="AJ1" s="12" t="s">
+      <c r="AK1" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="AK1" s="12" t="s">
+      <c r="AL1" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="AL1" s="12" t="s">
+      <c r="AM1" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="AM1" s="12" t="s">
+      <c r="AN1" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="AN1" s="12" t="s">
+      <c r="AO1" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="AO1" s="12" t="s">
+      <c r="AP1" s="10" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>87</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>89</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -1460,91 +1515,95 @@
         <v>98</v>
       </c>
       <c r="O2" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AG2" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="AG2" s="2" t="s">
+      <c r="AH2" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="AH2" s="2" t="s">
+      <c r="AI2" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="AI2" s="2" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AK2" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="AK2" s="2" t="s">
+      <c r="AL2" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="AL2" s="2" t="s">
+      <c r="AM2" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="AM2" s="2" t="s">
+      <c r="AN2" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="AN2" s="2" t="s">
+      <c r="AO2" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="AO2" s="2" t="s">
+      <c r="AP2" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="AP2" s="8" t="s">
+      <c r="AQ2" s="6" t="s">
         <v>106</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>